<commit_message>
Grade tables now also in stripped form for easier input.
</commit_message>
<xml_diff>
--- a/TestData/Vorlagen/Notenzeugnis/Notentabelle-12_SII.xlsx
+++ b/TestData/Vorlagen/Notenzeugnis/Notentabelle-12_SII.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
   <si>
     <r>
       <rPr>
@@ -600,7 +600,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -998,7 +998,9 @@
       <c r="AM9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
+      <c r="A10" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="7"/>
@@ -1041,7 +1043,9 @@
       <c r="AM10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
+      <c r="A11" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="7"/>
@@ -1084,7 +1088,9 @@
       <c r="AM11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
+      <c r="A12" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="7"/>
@@ -1127,7 +1133,9 @@
       <c r="AM12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
+      <c r="A13" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="7"/>
@@ -1170,7 +1178,9 @@
       <c r="AM13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
+      <c r="A14" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="7"/>
@@ -1213,7 +1223,9 @@
       <c r="AM14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
+      <c r="A15" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="7"/>
@@ -1256,7 +1268,9 @@
       <c r="AM15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
+      <c r="A16" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="7"/>
@@ -1299,7 +1313,9 @@
       <c r="AM16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6"/>
+      <c r="A17" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="7"/>
@@ -1342,7 +1358,9 @@
       <c r="AM17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6"/>
+      <c r="A18" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="7"/>
@@ -1385,7 +1403,9 @@
       <c r="AM18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6"/>
+      <c r="A19" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="7"/>
@@ -1428,7 +1448,9 @@
       <c r="AM19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6"/>
+      <c r="A20" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="7"/>
@@ -1471,7 +1493,9 @@
       <c r="AM20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6"/>
+      <c r="A21" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="7"/>
@@ -1514,7 +1538,9 @@
       <c r="AM21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6"/>
+      <c r="A22" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="7"/>
@@ -1557,7 +1583,9 @@
       <c r="AM22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6"/>
+      <c r="A23" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="7"/>
@@ -1600,7 +1628,9 @@
       <c r="AM23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
+      <c r="A24" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="7"/>
@@ -1643,7 +1673,9 @@
       <c r="AM24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6"/>
+      <c r="A25" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="7"/>
@@ -1686,7 +1718,9 @@
       <c r="AM25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
+      <c r="A26" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="7"/>
@@ -1729,7 +1763,9 @@
       <c r="AM26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6"/>
+      <c r="A27" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="7"/>
@@ -1772,7 +1808,9 @@
       <c r="AM27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
+      <c r="A28" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="7"/>
@@ -1815,7 +1853,9 @@
       <c r="AM28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6"/>
+      <c r="A29" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="7"/>
@@ -1858,7 +1898,9 @@
       <c r="AM29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6"/>
+      <c r="A30" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="7"/>
@@ -1901,7 +1943,9 @@
       <c r="AM30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6"/>
+      <c r="A31" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="7"/>
@@ -1944,7 +1988,9 @@
       <c r="AM31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6"/>
+      <c r="A32" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
       <c r="D32" s="7"/>
@@ -1987,7 +2033,9 @@
       <c r="AM32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6"/>
+      <c r="A33" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
       <c r="D33" s="7"/>
@@ -2030,7 +2078,9 @@
       <c r="AM33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6"/>
+      <c r="A34" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
       <c r="D34" s="7"/>
@@ -2073,7 +2123,9 @@
       <c r="AM34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6"/>
+      <c r="A35" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
       <c r="D35" s="7"/>
@@ -2116,7 +2168,9 @@
       <c r="AM35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6"/>
+      <c r="A36" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
       <c r="D36" s="7"/>
@@ -2159,7 +2213,9 @@
       <c r="AM36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6"/>
+      <c r="A37" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
       <c r="D37" s="7"/>
@@ -2202,7 +2258,9 @@
       <c r="AM37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6"/>
+      <c r="A38" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
       <c r="D38" s="7"/>
@@ -2245,7 +2303,9 @@
       <c r="AM38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6"/>
+      <c r="A39" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
       <c r="D39" s="7"/>
@@ -2288,7 +2348,9 @@
       <c r="AM39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6"/>
+      <c r="A40" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
       <c r="D40" s="7"/>
@@ -2331,7 +2393,9 @@
       <c r="AM40" s="22"/>
     </row>
     <row r="41" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6"/>
+      <c r="A41" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
       <c r="D41" s="7"/>
@@ -2374,7 +2438,9 @@
       <c r="AM41" s="22"/>
     </row>
     <row r="42" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6"/>
+      <c r="A42" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
       <c r="D42" s="7"/>
@@ -2417,7 +2483,9 @@
       <c r="AM42" s="22"/>
     </row>
     <row r="43" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6"/>
+      <c r="A43" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
       <c r="D43" s="7"/>
@@ -2460,7 +2528,9 @@
       <c r="AM43" s="22"/>
     </row>
     <row r="44" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6"/>
+      <c r="A44" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
       <c r="D44" s="7"/>
@@ -2503,7 +2573,9 @@
       <c r="AM44" s="22"/>
     </row>
     <row r="45" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6"/>
+      <c r="A45" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
       <c r="D45" s="7"/>
@@ -2546,7 +2618,9 @@
       <c r="AM45" s="22"/>
     </row>
     <row r="46" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6"/>
+      <c r="A46" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
       <c r="D46" s="7"/>
@@ -2589,7 +2663,9 @@
       <c r="AM46" s="22"/>
     </row>
     <row r="47" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6"/>
+      <c r="A47" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
       <c r="D47" s="7"/>
@@ -2632,7 +2708,9 @@
       <c r="AM47" s="22"/>
     </row>
     <row r="48" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6"/>
+      <c r="A48" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
       <c r="D48" s="7"/>
@@ -2675,7 +2753,9 @@
       <c r="AM48" s="22"/>
     </row>
     <row r="49" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6"/>
+      <c r="A49" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
       <c r="D49" s="7"/>
@@ -2718,7 +2798,9 @@
       <c r="AM49" s="22"/>
     </row>
     <row r="50" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="6"/>
+      <c r="A50" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
       <c r="D50" s="7"/>

</xml_diff>

<commit_message>
Replace school-class and stream strings by <Klass> instances for grade reports.
</commit_message>
<xml_diff>
--- a/TestData/Vorlagen/Notenzeugnis/Notentabelle-12_SII.xlsx
+++ b/TestData/Vorlagen/Notenzeugnis/Notentabelle-12_SII.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="66">
   <si>
     <r>
       <rPr>
@@ -118,25 +118,28 @@
     <t xml:space="preserve">Sp</t>
   </si>
   <si>
+    <t xml:space="preserve">AWT</t>
+  </si>
+  <si>
     <t xml:space="preserve">__Ku</t>
   </si>
   <si>
-    <t xml:space="preserve">Bb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sth</t>
+    <t xml:space="preserve">Bb_k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FK_k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kge_k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mal_k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pls_k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sth_k</t>
   </si>
   <si>
     <t xml:space="preserve">Eu</t>
@@ -194,6 +197,9 @@
   </si>
   <si>
     <t xml:space="preserve">Sport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arbeit-Wirtschaft-Technik</t>
   </si>
   <si>
     <t xml:space="preserve">Kunst</t>
@@ -313,7 +319,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,6 +366,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF4000"/>
         <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFDEDCE6"/>
       </patternFill>
     </fill>
     <fill>
@@ -423,7 +435,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -500,19 +512,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -541,7 +557,7 @@
       <rgbColor rgb="FFB47804"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF777777"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -596,11 +612,11 @@
   <dimension ref="A1:AM50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="P9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -775,145 +791,147 @@
         <v>15</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W6" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X6" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Z6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="AA6" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB6" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AE6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="AG6" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AI6" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AK6" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AL6" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AM6" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="94.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="7"/>
       <c r="E7" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
+      <c r="T7" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="U7" s="11"/>
       <c r="V7" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="W7" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="X7" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Y7" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="Z7" s="10"/>
       <c r="AA7" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AB7" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AC7" s="10"/>
       <c r="AD7" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="11"/>
       <c r="AG7" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AH7" s="11"/>
       <c r="AI7" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AJ7" s="11"/>
       <c r="AK7" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AL7" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AM7" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="8.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -954,7 +972,7 @@
     </row>
     <row r="9" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -974,8 +992,10 @@
       <c r="Q9" s="18"/>
       <c r="R9" s="18"/>
       <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="V9" s="19" t="str">
+      <c r="T9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V9" s="20" t="str">
         <f aca="false" t="array" ref="V9:V9">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W9:AE9,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -989,17 +1009,17 @@
       <c r="AD9" s="18"/>
       <c r="AE9" s="18"/>
       <c r="AG9" s="18"/>
-      <c r="AI9" s="20" t="e">
+      <c r="AI9" s="21" t="e">
         <f aca="false" t="array" ref="AI9:AI9">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E9:V9,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK9" s="21"/>
-      <c r="AL9" s="22"/>
-      <c r="AM9" s="22"/>
+      <c r="AK9" s="22"/>
+      <c r="AL9" s="23"/>
+      <c r="AM9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -1019,8 +1039,10 @@
       <c r="Q10" s="18"/>
       <c r="R10" s="18"/>
       <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="V10" s="19" t="str">
+      <c r="T10" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V10" s="20" t="str">
         <f aca="false" t="array" ref="V10:V10">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W10:AE10,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1034,17 +1056,17 @@
       <c r="AD10" s="18"/>
       <c r="AE10" s="18"/>
       <c r="AG10" s="18"/>
-      <c r="AI10" s="20" t="e">
+      <c r="AI10" s="21" t="e">
         <f aca="false" t="array" ref="AI10:AI10">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E10:V10,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK10" s="21"/>
-      <c r="AL10" s="22"/>
-      <c r="AM10" s="22"/>
+      <c r="AK10" s="22"/>
+      <c r="AL10" s="23"/>
+      <c r="AM10" s="23"/>
     </row>
     <row r="11" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -1064,8 +1086,10 @@
       <c r="Q11" s="18"/>
       <c r="R11" s="18"/>
       <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="V11" s="19" t="str">
+      <c r="T11" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V11" s="20" t="str">
         <f aca="false" t="array" ref="V11:V11">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W11:AE11,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1079,17 +1103,17 @@
       <c r="AD11" s="18"/>
       <c r="AE11" s="18"/>
       <c r="AG11" s="18"/>
-      <c r="AI11" s="20" t="e">
+      <c r="AI11" s="21" t="e">
         <f aca="false" t="array" ref="AI11:AI11">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E11:V11,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK11" s="21"/>
-      <c r="AL11" s="22"/>
-      <c r="AM11" s="22"/>
+      <c r="AK11" s="22"/>
+      <c r="AL11" s="23"/>
+      <c r="AM11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
@@ -1109,8 +1133,10 @@
       <c r="Q12" s="18"/>
       <c r="R12" s="18"/>
       <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="V12" s="19" t="str">
+      <c r="T12" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V12" s="20" t="str">
         <f aca="false" t="array" ref="V12:V12">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W12:AE12,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1124,17 +1150,17 @@
       <c r="AD12" s="18"/>
       <c r="AE12" s="18"/>
       <c r="AG12" s="18"/>
-      <c r="AI12" s="20" t="e">
+      <c r="AI12" s="21" t="e">
         <f aca="false" t="array" ref="AI12:AI12">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E12:V12,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK12" s="21"/>
-      <c r="AL12" s="22"/>
-      <c r="AM12" s="22"/>
+      <c r="AK12" s="22"/>
+      <c r="AL12" s="23"/>
+      <c r="AM12" s="23"/>
     </row>
     <row r="13" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -1154,8 +1180,10 @@
       <c r="Q13" s="18"/>
       <c r="R13" s="18"/>
       <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="V13" s="19" t="str">
+      <c r="T13" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V13" s="20" t="str">
         <f aca="false" t="array" ref="V13:V13">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W13:AE13,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1169,17 +1197,17 @@
       <c r="AD13" s="18"/>
       <c r="AE13" s="18"/>
       <c r="AG13" s="18"/>
-      <c r="AI13" s="20" t="e">
+      <c r="AI13" s="21" t="e">
         <f aca="false" t="array" ref="AI13:AI13">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E13:V13,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK13" s="21"/>
-      <c r="AL13" s="22"/>
-      <c r="AM13" s="22"/>
+      <c r="AK13" s="22"/>
+      <c r="AL13" s="23"/>
+      <c r="AM13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
@@ -1199,8 +1227,10 @@
       <c r="Q14" s="18"/>
       <c r="R14" s="18"/>
       <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="V14" s="19" t="str">
+      <c r="T14" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V14" s="20" t="str">
         <f aca="false" t="array" ref="V14:V14">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W14:AE14,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1214,17 +1244,17 @@
       <c r="AD14" s="18"/>
       <c r="AE14" s="18"/>
       <c r="AG14" s="18"/>
-      <c r="AI14" s="20" t="e">
+      <c r="AI14" s="21" t="e">
         <f aca="false" t="array" ref="AI14:AI14">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E14:V14,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK14" s="21"/>
-      <c r="AL14" s="22"/>
-      <c r="AM14" s="22"/>
+      <c r="AK14" s="22"/>
+      <c r="AL14" s="23"/>
+      <c r="AM14" s="23"/>
     </row>
     <row r="15" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -1244,8 +1274,10 @@
       <c r="Q15" s="18"/>
       <c r="R15" s="18"/>
       <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="V15" s="19" t="str">
+      <c r="T15" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V15" s="20" t="str">
         <f aca="false" t="array" ref="V15:V15">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W15:AE15,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1259,17 +1291,17 @@
       <c r="AD15" s="18"/>
       <c r="AE15" s="18"/>
       <c r="AG15" s="18"/>
-      <c r="AI15" s="20" t="e">
+      <c r="AI15" s="21" t="e">
         <f aca="false" t="array" ref="AI15:AI15">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E15:V15,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK15" s="21"/>
-      <c r="AL15" s="22"/>
-      <c r="AM15" s="22"/>
+      <c r="AK15" s="22"/>
+      <c r="AL15" s="23"/>
+      <c r="AM15" s="23"/>
     </row>
     <row r="16" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
@@ -1289,8 +1321,10 @@
       <c r="Q16" s="18"/>
       <c r="R16" s="18"/>
       <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="V16" s="19" t="str">
+      <c r="T16" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V16" s="20" t="str">
         <f aca="false" t="array" ref="V16:V16">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W16:AE16,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1304,17 +1338,17 @@
       <c r="AD16" s="18"/>
       <c r="AE16" s="18"/>
       <c r="AG16" s="18"/>
-      <c r="AI16" s="20" t="e">
+      <c r="AI16" s="21" t="e">
         <f aca="false" t="array" ref="AI16:AI16">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E16:V16,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK16" s="21"/>
-      <c r="AL16" s="22"/>
-      <c r="AM16" s="22"/>
+      <c r="AK16" s="22"/>
+      <c r="AL16" s="23"/>
+      <c r="AM16" s="23"/>
     </row>
     <row r="17" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -1334,8 +1368,10 @@
       <c r="Q17" s="18"/>
       <c r="R17" s="18"/>
       <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="V17" s="19" t="str">
+      <c r="T17" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V17" s="20" t="str">
         <f aca="false" t="array" ref="V17:V17">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W17:AE17,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1349,17 +1385,17 @@
       <c r="AD17" s="18"/>
       <c r="AE17" s="18"/>
       <c r="AG17" s="18"/>
-      <c r="AI17" s="20" t="e">
+      <c r="AI17" s="21" t="e">
         <f aca="false" t="array" ref="AI17:AI17">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E17:V17,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK17" s="21"/>
-      <c r="AL17" s="22"/>
-      <c r="AM17" s="22"/>
+      <c r="AK17" s="22"/>
+      <c r="AL17" s="23"/>
+      <c r="AM17" s="23"/>
     </row>
     <row r="18" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -1379,8 +1415,10 @@
       <c r="Q18" s="18"/>
       <c r="R18" s="18"/>
       <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="V18" s="19" t="str">
+      <c r="T18" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V18" s="20" t="str">
         <f aca="false" t="array" ref="V18:V18">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W18:AE18,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1394,17 +1432,17 @@
       <c r="AD18" s="18"/>
       <c r="AE18" s="18"/>
       <c r="AG18" s="18"/>
-      <c r="AI18" s="20" t="e">
+      <c r="AI18" s="21" t="e">
         <f aca="false" t="array" ref="AI18:AI18">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E18:V18,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK18" s="21"/>
-      <c r="AL18" s="22"/>
-      <c r="AM18" s="22"/>
+      <c r="AK18" s="22"/>
+      <c r="AL18" s="23"/>
+      <c r="AM18" s="23"/>
     </row>
     <row r="19" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -1424,8 +1462,10 @@
       <c r="Q19" s="18"/>
       <c r="R19" s="18"/>
       <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="V19" s="19" t="str">
+      <c r="T19" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V19" s="20" t="str">
         <f aca="false" t="array" ref="V19:V19">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W19:AE19,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1439,17 +1479,17 @@
       <c r="AD19" s="18"/>
       <c r="AE19" s="18"/>
       <c r="AG19" s="18"/>
-      <c r="AI19" s="20" t="e">
+      <c r="AI19" s="21" t="e">
         <f aca="false" t="array" ref="AI19:AI19">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E19:V19,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK19" s="21"/>
-      <c r="AL19" s="22"/>
-      <c r="AM19" s="22"/>
+      <c r="AK19" s="22"/>
+      <c r="AL19" s="23"/>
+      <c r="AM19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -1469,8 +1509,10 @@
       <c r="Q20" s="18"/>
       <c r="R20" s="18"/>
       <c r="S20" s="18"/>
-      <c r="T20" s="18"/>
-      <c r="V20" s="19" t="str">
+      <c r="T20" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V20" s="20" t="str">
         <f aca="false" t="array" ref="V20:V20">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W20:AE20,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1484,17 +1526,17 @@
       <c r="AD20" s="18"/>
       <c r="AE20" s="18"/>
       <c r="AG20" s="18"/>
-      <c r="AI20" s="20" t="e">
+      <c r="AI20" s="21" t="e">
         <f aca="false" t="array" ref="AI20:AI20">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E20:V20,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK20" s="21"/>
-      <c r="AL20" s="22"/>
-      <c r="AM20" s="22"/>
+      <c r="AK20" s="22"/>
+      <c r="AL20" s="23"/>
+      <c r="AM20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -1514,8 +1556,10 @@
       <c r="Q21" s="18"/>
       <c r="R21" s="18"/>
       <c r="S21" s="18"/>
-      <c r="T21" s="18"/>
-      <c r="V21" s="19" t="str">
+      <c r="T21" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V21" s="20" t="str">
         <f aca="false" t="array" ref="V21:V21">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W21:AE21,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1529,17 +1573,17 @@
       <c r="AD21" s="18"/>
       <c r="AE21" s="18"/>
       <c r="AG21" s="18"/>
-      <c r="AI21" s="20" t="e">
+      <c r="AI21" s="21" t="e">
         <f aca="false" t="array" ref="AI21:AI21">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E21:V21,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK21" s="21"/>
-      <c r="AL21" s="22"/>
-      <c r="AM21" s="22"/>
+      <c r="AK21" s="22"/>
+      <c r="AL21" s="23"/>
+      <c r="AM21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -1559,8 +1603,10 @@
       <c r="Q22" s="18"/>
       <c r="R22" s="18"/>
       <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
-      <c r="V22" s="19" t="str">
+      <c r="T22" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V22" s="20" t="str">
         <f aca="false" t="array" ref="V22:V22">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W22:AE22,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1574,17 +1620,17 @@
       <c r="AD22" s="18"/>
       <c r="AE22" s="18"/>
       <c r="AG22" s="18"/>
-      <c r="AI22" s="20" t="e">
+      <c r="AI22" s="21" t="e">
         <f aca="false" t="array" ref="AI22:AI22">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E22:V22,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK22" s="21"/>
-      <c r="AL22" s="22"/>
-      <c r="AM22" s="22"/>
+      <c r="AK22" s="22"/>
+      <c r="AL22" s="23"/>
+      <c r="AM22" s="23"/>
     </row>
     <row r="23" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -1604,8 +1650,10 @@
       <c r="Q23" s="18"/>
       <c r="R23" s="18"/>
       <c r="S23" s="18"/>
-      <c r="T23" s="18"/>
-      <c r="V23" s="19" t="str">
+      <c r="T23" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V23" s="20" t="str">
         <f aca="false" t="array" ref="V23:V23">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W23:AE23,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1619,17 +1667,17 @@
       <c r="AD23" s="18"/>
       <c r="AE23" s="18"/>
       <c r="AG23" s="18"/>
-      <c r="AI23" s="20" t="e">
+      <c r="AI23" s="21" t="e">
         <f aca="false" t="array" ref="AI23:AI23">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E23:V23,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK23" s="21"/>
-      <c r="AL23" s="22"/>
-      <c r="AM23" s="22"/>
+      <c r="AK23" s="22"/>
+      <c r="AL23" s="23"/>
+      <c r="AM23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
@@ -1649,8 +1697,10 @@
       <c r="Q24" s="18"/>
       <c r="R24" s="18"/>
       <c r="S24" s="18"/>
-      <c r="T24" s="18"/>
-      <c r="V24" s="19" t="str">
+      <c r="T24" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V24" s="20" t="str">
         <f aca="false" t="array" ref="V24:V24">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W24:AE24,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1664,17 +1714,17 @@
       <c r="AD24" s="18"/>
       <c r="AE24" s="18"/>
       <c r="AG24" s="18"/>
-      <c r="AI24" s="20" t="e">
+      <c r="AI24" s="21" t="e">
         <f aca="false" t="array" ref="AI24:AI24">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E24:V24,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK24" s="21"/>
-      <c r="AL24" s="22"/>
-      <c r="AM24" s="22"/>
+      <c r="AK24" s="22"/>
+      <c r="AL24" s="23"/>
+      <c r="AM24" s="23"/>
     </row>
     <row r="25" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -1694,8 +1744,10 @@
       <c r="Q25" s="18"/>
       <c r="R25" s="18"/>
       <c r="S25" s="18"/>
-      <c r="T25" s="18"/>
-      <c r="V25" s="19" t="str">
+      <c r="T25" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V25" s="20" t="str">
         <f aca="false" t="array" ref="V25:V25">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W25:AE25,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1709,17 +1761,17 @@
       <c r="AD25" s="18"/>
       <c r="AE25" s="18"/>
       <c r="AG25" s="18"/>
-      <c r="AI25" s="20" t="e">
+      <c r="AI25" s="21" t="e">
         <f aca="false" t="array" ref="AI25:AI25">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E25:V25,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK25" s="21"/>
-      <c r="AL25" s="22"/>
-      <c r="AM25" s="22"/>
+      <c r="AK25" s="22"/>
+      <c r="AL25" s="23"/>
+      <c r="AM25" s="23"/>
     </row>
     <row r="26" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -1739,8 +1791,10 @@
       <c r="Q26" s="18"/>
       <c r="R26" s="18"/>
       <c r="S26" s="18"/>
-      <c r="T26" s="18"/>
-      <c r="V26" s="19" t="str">
+      <c r="T26" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V26" s="20" t="str">
         <f aca="false" t="array" ref="V26:V26">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W26:AE26,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1754,17 +1808,17 @@
       <c r="AD26" s="18"/>
       <c r="AE26" s="18"/>
       <c r="AG26" s="18"/>
-      <c r="AI26" s="20" t="e">
+      <c r="AI26" s="21" t="e">
         <f aca="false" t="array" ref="AI26:AI26">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E26:V26,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK26" s="21"/>
-      <c r="AL26" s="22"/>
-      <c r="AM26" s="22"/>
+      <c r="AK26" s="22"/>
+      <c r="AL26" s="23"/>
+      <c r="AM26" s="23"/>
     </row>
     <row r="27" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -1784,8 +1838,10 @@
       <c r="Q27" s="18"/>
       <c r="R27" s="18"/>
       <c r="S27" s="18"/>
-      <c r="T27" s="18"/>
-      <c r="V27" s="19" t="str">
+      <c r="T27" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V27" s="20" t="str">
         <f aca="false" t="array" ref="V27:V27">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W27:AE27,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1799,17 +1855,17 @@
       <c r="AD27" s="18"/>
       <c r="AE27" s="18"/>
       <c r="AG27" s="18"/>
-      <c r="AI27" s="20" t="e">
+      <c r="AI27" s="21" t="e">
         <f aca="false" t="array" ref="AI27:AI27">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E27:V27,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK27" s="21"/>
-      <c r="AL27" s="22"/>
-      <c r="AM27" s="22"/>
+      <c r="AK27" s="22"/>
+      <c r="AL27" s="23"/>
+      <c r="AM27" s="23"/>
     </row>
     <row r="28" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
@@ -1829,8 +1885,10 @@
       <c r="Q28" s="18"/>
       <c r="R28" s="18"/>
       <c r="S28" s="18"/>
-      <c r="T28" s="18"/>
-      <c r="V28" s="19" t="str">
+      <c r="T28" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V28" s="20" t="str">
         <f aca="false" t="array" ref="V28:V28">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W28:AE28,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1844,17 +1902,17 @@
       <c r="AD28" s="18"/>
       <c r="AE28" s="18"/>
       <c r="AG28" s="18"/>
-      <c r="AI28" s="20" t="e">
+      <c r="AI28" s="21" t="e">
         <f aca="false" t="array" ref="AI28:AI28">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E28:V28,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK28" s="21"/>
-      <c r="AL28" s="22"/>
-      <c r="AM28" s="22"/>
+      <c r="AK28" s="22"/>
+      <c r="AL28" s="23"/>
+      <c r="AM28" s="23"/>
     </row>
     <row r="29" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -1874,8 +1932,10 @@
       <c r="Q29" s="18"/>
       <c r="R29" s="18"/>
       <c r="S29" s="18"/>
-      <c r="T29" s="18"/>
-      <c r="V29" s="19" t="str">
+      <c r="T29" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V29" s="20" t="str">
         <f aca="false" t="array" ref="V29:V29">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W29:AE29,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1889,17 +1949,17 @@
       <c r="AD29" s="18"/>
       <c r="AE29" s="18"/>
       <c r="AG29" s="18"/>
-      <c r="AI29" s="20" t="e">
+      <c r="AI29" s="21" t="e">
         <f aca="false" t="array" ref="AI29:AI29">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E29:V29,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK29" s="21"/>
-      <c r="AL29" s="22"/>
-      <c r="AM29" s="22"/>
+      <c r="AK29" s="22"/>
+      <c r="AL29" s="23"/>
+      <c r="AM29" s="23"/>
     </row>
     <row r="30" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
@@ -1919,8 +1979,10 @@
       <c r="Q30" s="18"/>
       <c r="R30" s="18"/>
       <c r="S30" s="18"/>
-      <c r="T30" s="18"/>
-      <c r="V30" s="19" t="str">
+      <c r="T30" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V30" s="20" t="str">
         <f aca="false" t="array" ref="V30:V30">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W30:AE30,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1934,17 +1996,17 @@
       <c r="AD30" s="18"/>
       <c r="AE30" s="18"/>
       <c r="AG30" s="18"/>
-      <c r="AI30" s="20" t="e">
+      <c r="AI30" s="21" t="e">
         <f aca="false" t="array" ref="AI30:AI30">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E30:V30,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK30" s="21"/>
-      <c r="AL30" s="22"/>
-      <c r="AM30" s="22"/>
+      <c r="AK30" s="22"/>
+      <c r="AL30" s="23"/>
+      <c r="AM30" s="23"/>
     </row>
     <row r="31" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -1964,8 +2026,10 @@
       <c r="Q31" s="18"/>
       <c r="R31" s="18"/>
       <c r="S31" s="18"/>
-      <c r="T31" s="18"/>
-      <c r="V31" s="19" t="str">
+      <c r="T31" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V31" s="20" t="str">
         <f aca="false" t="array" ref="V31:V31">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W31:AE31,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -1979,17 +2043,17 @@
       <c r="AD31" s="18"/>
       <c r="AE31" s="18"/>
       <c r="AG31" s="18"/>
-      <c r="AI31" s="20" t="e">
+      <c r="AI31" s="21" t="e">
         <f aca="false" t="array" ref="AI31:AI31">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E31:V31,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK31" s="21"/>
-      <c r="AL31" s="22"/>
-      <c r="AM31" s="22"/>
+      <c r="AK31" s="22"/>
+      <c r="AL31" s="23"/>
+      <c r="AM31" s="23"/>
     </row>
     <row r="32" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -2009,8 +2073,10 @@
       <c r="Q32" s="18"/>
       <c r="R32" s="18"/>
       <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="V32" s="19" t="str">
+      <c r="T32" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V32" s="20" t="str">
         <f aca="false" t="array" ref="V32:V32">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W32:AE32,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2024,17 +2090,17 @@
       <c r="AD32" s="18"/>
       <c r="AE32" s="18"/>
       <c r="AG32" s="18"/>
-      <c r="AI32" s="20" t="e">
+      <c r="AI32" s="21" t="e">
         <f aca="false" t="array" ref="AI32:AI32">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E32:V32,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK32" s="21"/>
-      <c r="AL32" s="22"/>
-      <c r="AM32" s="22"/>
+      <c r="AK32" s="22"/>
+      <c r="AL32" s="23"/>
+      <c r="AM32" s="23"/>
     </row>
     <row r="33" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -2054,8 +2120,10 @@
       <c r="Q33" s="18"/>
       <c r="R33" s="18"/>
       <c r="S33" s="18"/>
-      <c r="T33" s="18"/>
-      <c r="V33" s="19" t="str">
+      <c r="T33" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V33" s="20" t="str">
         <f aca="false" t="array" ref="V33:V33">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W33:AE33,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2069,17 +2137,17 @@
       <c r="AD33" s="18"/>
       <c r="AE33" s="18"/>
       <c r="AG33" s="18"/>
-      <c r="AI33" s="20" t="e">
+      <c r="AI33" s="21" t="e">
         <f aca="false" t="array" ref="AI33:AI33">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E33:V33,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK33" s="21"/>
-      <c r="AL33" s="22"/>
-      <c r="AM33" s="22"/>
+      <c r="AK33" s="22"/>
+      <c r="AL33" s="23"/>
+      <c r="AM33" s="23"/>
     </row>
     <row r="34" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -2099,8 +2167,10 @@
       <c r="Q34" s="18"/>
       <c r="R34" s="18"/>
       <c r="S34" s="18"/>
-      <c r="T34" s="18"/>
-      <c r="V34" s="19" t="str">
+      <c r="T34" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V34" s="20" t="str">
         <f aca="false" t="array" ref="V34:V34">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W34:AE34,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2114,17 +2184,17 @@
       <c r="AD34" s="18"/>
       <c r="AE34" s="18"/>
       <c r="AG34" s="18"/>
-      <c r="AI34" s="20" t="e">
+      <c r="AI34" s="21" t="e">
         <f aca="false" t="array" ref="AI34:AI34">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E34:V34,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK34" s="21"/>
-      <c r="AL34" s="22"/>
-      <c r="AM34" s="22"/>
+      <c r="AK34" s="22"/>
+      <c r="AL34" s="23"/>
+      <c r="AM34" s="23"/>
     </row>
     <row r="35" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -2144,8 +2214,10 @@
       <c r="Q35" s="18"/>
       <c r="R35" s="18"/>
       <c r="S35" s="18"/>
-      <c r="T35" s="18"/>
-      <c r="V35" s="19" t="str">
+      <c r="T35" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V35" s="20" t="str">
         <f aca="false" t="array" ref="V35:V35">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W35:AE35,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2159,17 +2231,17 @@
       <c r="AD35" s="18"/>
       <c r="AE35" s="18"/>
       <c r="AG35" s="18"/>
-      <c r="AI35" s="20" t="e">
+      <c r="AI35" s="21" t="e">
         <f aca="false" t="array" ref="AI35:AI35">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E35:V35,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK35" s="21"/>
-      <c r="AL35" s="22"/>
-      <c r="AM35" s="22"/>
+      <c r="AK35" s="22"/>
+      <c r="AL35" s="23"/>
+      <c r="AM35" s="23"/>
     </row>
     <row r="36" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
@@ -2189,8 +2261,10 @@
       <c r="Q36" s="18"/>
       <c r="R36" s="18"/>
       <c r="S36" s="18"/>
-      <c r="T36" s="18"/>
-      <c r="V36" s="19" t="str">
+      <c r="T36" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V36" s="20" t="str">
         <f aca="false" t="array" ref="V36:V36">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W36:AE36,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2204,17 +2278,17 @@
       <c r="AD36" s="18"/>
       <c r="AE36" s="18"/>
       <c r="AG36" s="18"/>
-      <c r="AI36" s="20" t="e">
+      <c r="AI36" s="21" t="e">
         <f aca="false" t="array" ref="AI36:AI36">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E36:V36,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK36" s="21"/>
-      <c r="AL36" s="22"/>
-      <c r="AM36" s="22"/>
+      <c r="AK36" s="22"/>
+      <c r="AL36" s="23"/>
+      <c r="AM36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
@@ -2234,8 +2308,10 @@
       <c r="Q37" s="18"/>
       <c r="R37" s="18"/>
       <c r="S37" s="18"/>
-      <c r="T37" s="18"/>
-      <c r="V37" s="19" t="str">
+      <c r="T37" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V37" s="20" t="str">
         <f aca="false" t="array" ref="V37:V37">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W37:AE37,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2249,17 +2325,17 @@
       <c r="AD37" s="18"/>
       <c r="AE37" s="18"/>
       <c r="AG37" s="18"/>
-      <c r="AI37" s="20" t="e">
+      <c r="AI37" s="21" t="e">
         <f aca="false" t="array" ref="AI37:AI37">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E37:V37,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK37" s="21"/>
-      <c r="AL37" s="22"/>
-      <c r="AM37" s="22"/>
+      <c r="AK37" s="22"/>
+      <c r="AL37" s="23"/>
+      <c r="AM37" s="23"/>
     </row>
     <row r="38" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
@@ -2279,8 +2355,10 @@
       <c r="Q38" s="18"/>
       <c r="R38" s="18"/>
       <c r="S38" s="18"/>
-      <c r="T38" s="18"/>
-      <c r="V38" s="19" t="str">
+      <c r="T38" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V38" s="20" t="str">
         <f aca="false" t="array" ref="V38:V38">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W38:AE38,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2294,17 +2372,17 @@
       <c r="AD38" s="18"/>
       <c r="AE38" s="18"/>
       <c r="AG38" s="18"/>
-      <c r="AI38" s="20" t="e">
+      <c r="AI38" s="21" t="e">
         <f aca="false" t="array" ref="AI38:AI38">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E38:V38,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK38" s="21"/>
-      <c r="AL38" s="22"/>
-      <c r="AM38" s="22"/>
+      <c r="AK38" s="22"/>
+      <c r="AL38" s="23"/>
+      <c r="AM38" s="23"/>
     </row>
     <row r="39" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -2324,8 +2402,10 @@
       <c r="Q39" s="18"/>
       <c r="R39" s="18"/>
       <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="V39" s="19" t="str">
+      <c r="T39" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V39" s="20" t="str">
         <f aca="false" t="array" ref="V39:V39">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W39:AE39,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2339,17 +2419,17 @@
       <c r="AD39" s="18"/>
       <c r="AE39" s="18"/>
       <c r="AG39" s="18"/>
-      <c r="AI39" s="20" t="e">
+      <c r="AI39" s="21" t="e">
         <f aca="false" t="array" ref="AI39:AI39">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E39:V39,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK39" s="21"/>
-      <c r="AL39" s="22"/>
-      <c r="AM39" s="22"/>
+      <c r="AK39" s="22"/>
+      <c r="AL39" s="23"/>
+      <c r="AM39" s="23"/>
     </row>
     <row r="40" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
@@ -2369,8 +2449,10 @@
       <c r="Q40" s="18"/>
       <c r="R40" s="18"/>
       <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
-      <c r="V40" s="19" t="str">
+      <c r="T40" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V40" s="20" t="str">
         <f aca="false" t="array" ref="V40:V40">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W40:AE40,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2384,17 +2466,17 @@
       <c r="AD40" s="18"/>
       <c r="AE40" s="18"/>
       <c r="AG40" s="18"/>
-      <c r="AI40" s="20" t="e">
+      <c r="AI40" s="21" t="e">
         <f aca="false" t="array" ref="AI40:AI40">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E40:V40,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK40" s="21"/>
-      <c r="AL40" s="22"/>
-      <c r="AM40" s="22"/>
+      <c r="AK40" s="22"/>
+      <c r="AL40" s="23"/>
+      <c r="AM40" s="23"/>
     </row>
     <row r="41" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -2414,8 +2496,10 @@
       <c r="Q41" s="18"/>
       <c r="R41" s="18"/>
       <c r="S41" s="18"/>
-      <c r="T41" s="18"/>
-      <c r="V41" s="19" t="str">
+      <c r="T41" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V41" s="20" t="str">
         <f aca="false" t="array" ref="V41:V41">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W41:AE41,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2429,17 +2513,17 @@
       <c r="AD41" s="18"/>
       <c r="AE41" s="18"/>
       <c r="AG41" s="18"/>
-      <c r="AI41" s="20" t="e">
+      <c r="AI41" s="21" t="e">
         <f aca="false" t="array" ref="AI41:AI41">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E41:V41,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK41" s="21"/>
-      <c r="AL41" s="22"/>
-      <c r="AM41" s="22"/>
+      <c r="AK41" s="22"/>
+      <c r="AL41" s="23"/>
+      <c r="AM41" s="23"/>
     </row>
     <row r="42" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
@@ -2459,8 +2543,10 @@
       <c r="Q42" s="18"/>
       <c r="R42" s="18"/>
       <c r="S42" s="18"/>
-      <c r="T42" s="18"/>
-      <c r="V42" s="19" t="str">
+      <c r="T42" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V42" s="20" t="str">
         <f aca="false" t="array" ref="V42:V42">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W42:AE42,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2474,17 +2560,17 @@
       <c r="AD42" s="18"/>
       <c r="AE42" s="18"/>
       <c r="AG42" s="18"/>
-      <c r="AI42" s="20" t="e">
+      <c r="AI42" s="21" t="e">
         <f aca="false" t="array" ref="AI42:AI42">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E42:V42,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK42" s="21"/>
-      <c r="AL42" s="22"/>
-      <c r="AM42" s="22"/>
+      <c r="AK42" s="22"/>
+      <c r="AL42" s="23"/>
+      <c r="AM42" s="23"/>
     </row>
     <row r="43" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
@@ -2504,8 +2590,10 @@
       <c r="Q43" s="18"/>
       <c r="R43" s="18"/>
       <c r="S43" s="18"/>
-      <c r="T43" s="18"/>
-      <c r="V43" s="19" t="str">
+      <c r="T43" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V43" s="20" t="str">
         <f aca="false" t="array" ref="V43:V43">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W43:AE43,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2519,17 +2607,17 @@
       <c r="AD43" s="18"/>
       <c r="AE43" s="18"/>
       <c r="AG43" s="18"/>
-      <c r="AI43" s="20" t="e">
+      <c r="AI43" s="21" t="e">
         <f aca="false" t="array" ref="AI43:AI43">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E43:V43,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK43" s="21"/>
-      <c r="AL43" s="22"/>
-      <c r="AM43" s="22"/>
+      <c r="AK43" s="22"/>
+      <c r="AL43" s="23"/>
+      <c r="AM43" s="23"/>
     </row>
     <row r="44" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
@@ -2549,8 +2637,10 @@
       <c r="Q44" s="18"/>
       <c r="R44" s="18"/>
       <c r="S44" s="18"/>
-      <c r="T44" s="18"/>
-      <c r="V44" s="19" t="str">
+      <c r="T44" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V44" s="20" t="str">
         <f aca="false" t="array" ref="V44:V44">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W44:AE44,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2564,17 +2654,17 @@
       <c r="AD44" s="18"/>
       <c r="AE44" s="18"/>
       <c r="AG44" s="18"/>
-      <c r="AI44" s="20" t="e">
+      <c r="AI44" s="21" t="e">
         <f aca="false" t="array" ref="AI44:AI44">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E44:V44,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK44" s="21"/>
-      <c r="AL44" s="22"/>
-      <c r="AM44" s="22"/>
+      <c r="AK44" s="22"/>
+      <c r="AL44" s="23"/>
+      <c r="AM44" s="23"/>
     </row>
     <row r="45" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
@@ -2594,8 +2684,10 @@
       <c r="Q45" s="18"/>
       <c r="R45" s="18"/>
       <c r="S45" s="18"/>
-      <c r="T45" s="18"/>
-      <c r="V45" s="19" t="str">
+      <c r="T45" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V45" s="20" t="str">
         <f aca="false" t="array" ref="V45:V45">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W45:AE45,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2609,17 +2701,17 @@
       <c r="AD45" s="18"/>
       <c r="AE45" s="18"/>
       <c r="AG45" s="18"/>
-      <c r="AI45" s="20" t="e">
+      <c r="AI45" s="21" t="e">
         <f aca="false" t="array" ref="AI45:AI45">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E45:V45,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK45" s="21"/>
-      <c r="AL45" s="22"/>
-      <c r="AM45" s="22"/>
+      <c r="AK45" s="22"/>
+      <c r="AL45" s="23"/>
+      <c r="AM45" s="23"/>
     </row>
     <row r="46" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
@@ -2639,8 +2731,10 @@
       <c r="Q46" s="18"/>
       <c r="R46" s="18"/>
       <c r="S46" s="18"/>
-      <c r="T46" s="18"/>
-      <c r="V46" s="19" t="str">
+      <c r="T46" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V46" s="20" t="str">
         <f aca="false" t="array" ref="V46:V46">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W46:AE46,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2654,17 +2748,17 @@
       <c r="AD46" s="18"/>
       <c r="AE46" s="18"/>
       <c r="AG46" s="18"/>
-      <c r="AI46" s="20" t="e">
+      <c r="AI46" s="21" t="e">
         <f aca="false" t="array" ref="AI46:AI46">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E46:V46,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK46" s="21"/>
-      <c r="AL46" s="22"/>
-      <c r="AM46" s="22"/>
+      <c r="AK46" s="22"/>
+      <c r="AL46" s="23"/>
+      <c r="AM46" s="23"/>
     </row>
     <row r="47" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
@@ -2684,8 +2778,10 @@
       <c r="Q47" s="18"/>
       <c r="R47" s="18"/>
       <c r="S47" s="18"/>
-      <c r="T47" s="18"/>
-      <c r="V47" s="19" t="str">
+      <c r="T47" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V47" s="20" t="str">
         <f aca="false" t="array" ref="V47:V47">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W47:AE47,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2699,17 +2795,17 @@
       <c r="AD47" s="18"/>
       <c r="AE47" s="18"/>
       <c r="AG47" s="18"/>
-      <c r="AI47" s="20" t="e">
+      <c r="AI47" s="21" t="e">
         <f aca="false" t="array" ref="AI47:AI47">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E47:V47,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK47" s="21"/>
-      <c r="AL47" s="22"/>
-      <c r="AM47" s="22"/>
+      <c r="AK47" s="22"/>
+      <c r="AL47" s="23"/>
+      <c r="AM47" s="23"/>
     </row>
     <row r="48" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
@@ -2729,8 +2825,10 @@
       <c r="Q48" s="18"/>
       <c r="R48" s="18"/>
       <c r="S48" s="18"/>
-      <c r="T48" s="18"/>
-      <c r="V48" s="19" t="str">
+      <c r="T48" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V48" s="20" t="str">
         <f aca="false" t="array" ref="V48:V48">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W48:AE48,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2744,17 +2842,17 @@
       <c r="AD48" s="18"/>
       <c r="AE48" s="18"/>
       <c r="AG48" s="18"/>
-      <c r="AI48" s="20" t="e">
+      <c r="AI48" s="21" t="e">
         <f aca="false" t="array" ref="AI48:AI48">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E48:V48,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK48" s="21"/>
-      <c r="AL48" s="22"/>
-      <c r="AM48" s="22"/>
+      <c r="AK48" s="22"/>
+      <c r="AL48" s="23"/>
+      <c r="AM48" s="23"/>
     </row>
     <row r="49" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
@@ -2774,8 +2872,10 @@
       <c r="Q49" s="18"/>
       <c r="R49" s="18"/>
       <c r="S49" s="18"/>
-      <c r="T49" s="18"/>
-      <c r="V49" s="19" t="str">
+      <c r="T49" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V49" s="20" t="str">
         <f aca="false" t="array" ref="V49:V49">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W49:AE49,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2789,17 +2889,17 @@
       <c r="AD49" s="18"/>
       <c r="AE49" s="18"/>
       <c r="AG49" s="18"/>
-      <c r="AI49" s="20" t="e">
+      <c r="AI49" s="21" t="e">
         <f aca="false" t="array" ref="AI49:AI49">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E49:V49,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK49" s="21"/>
-      <c r="AL49" s="22"/>
-      <c r="AM49" s="22"/>
+      <c r="AK49" s="22"/>
+      <c r="AL49" s="23"/>
+      <c r="AM49" s="23"/>
     </row>
     <row r="50" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
@@ -2819,8 +2919,10 @@
       <c r="Q50" s="18"/>
       <c r="R50" s="18"/>
       <c r="S50" s="18"/>
-      <c r="T50" s="18"/>
-      <c r="V50" s="19" t="str">
+      <c r="T50" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V50" s="20" t="str">
         <f aca="false" t="array" ref="V50:V50">IFERROR(TEXT(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(W50:AE50,"-",""),"+","")),"")),"00"),"*")</f>
         <v>*</v>
       </c>
@@ -2834,19 +2936,19 @@
       <c r="AD50" s="18"/>
       <c r="AE50" s="18"/>
       <c r="AG50" s="18"/>
-      <c r="AI50" s="20" t="e">
+      <c r="AI50" s="21" t="e">
         <f aca="false" t="array" ref="AI50:AI50">ROUND(AVERAGE(IFERROR(_xlfn.NUMBERVALUE(SUBSTITUTE(SUBSTITUTE(E50:V50,"-",""),"+","")),"")),2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK50" s="21"/>
-      <c r="AL50" s="22"/>
-      <c r="AM50" s="22"/>
+      <c r="AK50" s="22"/>
+      <c r="AL50" s="23"/>
+      <c r="AM50" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AI9:AI50" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -2859,7 +2961,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E9:T50 W9:AE50 AG9:AG50" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E9:S50 W9:AE50 AG9:AG50" type="list">
       <formula1>"15,14,13,12,11,10,09,08,07,06,05,04,03,02,01,00,nb,nt,t,*"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2868,6 +2970,10 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V9:V50" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T9:T50" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>